<commit_message>
Fundamentals Version 2: - fundamentals.c [NEW COMMENTS AND CODE FOR V2] - fundamentals-test-cases.xlsx [NEW TEST CASES FOR V2] - REMOVED fundamentals-test-cases.png - ADDED        - fundamentals-V1-test-cases.png        - fundamentals-V2-test-cases.png        - fundamentals-testing.txt [RAW TEXT OF PROGRAM OUTPUT TO TESTS]
</commit_message>
<xml_diff>
--- a/fundamentals-test-cases.xlsx
+++ b/fundamentals-test-cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seneca\CPR101\CPR101-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9594769B-644A-4492-93B5-1C984C06E1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315CD049-326E-4165-9D56-D1B9CA53EE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,7 +520,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{EA807800-7D99-42C2-8FA7-105696568FFD}">
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{EA807800-7D99-42C2-8FA7-105696568FFD}">
       <text>
         <r>
           <rPr>
@@ -564,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{6523EF89-7C7C-41DC-B9D8-92708814E2E3}">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{6523EF89-7C7C-41DC-B9D8-92708814E2E3}">
       <text>
         <r>
           <rPr>
@@ -629,7 +629,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{4630BF63-60C7-42F9-9C60-EF9CD44B688A}">
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{4630BF63-60C7-42F9-9C60-EF9CD44B688A}">
       <text>
         <r>
           <rPr>
@@ -655,7 +655,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{A8EDB628-DA3F-4BA1-A578-480C70A6FC27}">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{A8EDB628-DA3F-4BA1-A578-480C70A6FC27}">
       <text>
         <r>
           <rPr>
@@ -700,7 +700,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{A6607402-9B3D-4194-8CA9-39747FF47C55}">
+    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{A6607402-9B3D-4194-8CA9-39747FF47C55}">
       <text>
         <r>
           <rPr>
@@ -724,7 +724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
       <text>
         <r>
           <rPr>
@@ -747,7 +747,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
       <text>
         <r>
           <rPr>
@@ -789,7 +789,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
   <si>
     <t>Comments</t>
   </si>
@@ -1009,12 +1009,94 @@
     <t>buffer1 = "Hello World"
 numInput = "11"</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+Program is running as intended with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>intended input</t>
+    </r>
+  </si>
+  <si>
+    <t>The length of 'Hello World' is 11 characters</t>
+  </si>
+  <si>
+    <t>+Program handles a min length string without error</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>"Hello World"</t>
+  </si>
+  <si>
+    <t>The length of '' is 0 characters
+OR
+Error indicating a 0 length string and reprompt</t>
+  </si>
+  <si>
+    <t>+Program handles a max length string without error</t>
+  </si>
+  <si>
+    <t>"1234567890123456789023456789012345678901234567890123456789012345678901234567890"</t>
+  </si>
+  <si>
+    <t>The length of '1234567890123456789023456789012345678901234567890123456789012345678901234567890' is 80 characters</t>
+  </si>
+  <si>
+    <t>The length of '123456789012345678902345678901234567890123456789012345678901234567890123456789' is 78 characters
+Type a string (q - to quit):
+The length of '' is 0 characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+Program exits with 'Q'
+</t>
+  </si>
+  <si>
+    <t>+Program exits with 'q'</t>
+  </si>
+  <si>
+    <t>Program lost the last character and also overflowed. The reason is that the null terminator that is put in by fgets() overflowed the string. The final char '0' was overwritten by the manual null termination added and thus it interpreted the input as two strings, one being the original text missing the final char and an "empty" string with only the null terminator.
+Recommended Fix: Fixes for this issue are identical to ones mentioned in Version 1. Namely, start using safer input methods such as sscanf() and have the buffer be 1 larger than the max size. 
+This issue would obviously not change if the program was given a blatantly too large string, and as such I have ommited testing for that case.</t>
+  </si>
+  <si>
+    <t>"Q"</t>
+  </si>
+  <si>
+    <t>"q"</t>
+  </si>
+  <si>
+    <t>Program exits</t>
+  </si>
+  <si>
+    <t>The length of 'Q' is 1 characters</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1104,6 +1186,12 @@
       <b/>
       <i/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1263,7 +1351,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1322,6 +1410,12 @@
     <xf numFmtId="14" fontId="14" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1334,10 +1428,7 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1643,10 +1734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1660,7 +1751,7 @@
     <col min="7" max="7" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1668,23 +1759,23 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>Fundamentals</v>
       </c>
-      <c r="C1" s="22" t="str">
+      <c r="C1" s="24" t="str">
         <f ca="1">"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As Fundamentals_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
@@ -1796,10 +1887,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="12" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1845,7 +1936,7 @@
       <c r="A10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="21" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1868,7 +1959,7 @@
       <c r="A11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1891,7 +1982,7 @@
       <c r="A12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="21" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1905,13 +1996,13 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="8" t="s">
         <v>5</v>
       </c>
@@ -1942,79 +2033,149 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
+    <row r="15" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
+      <c r="F15" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
+      <c r="F16" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="331.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="13"/>
+      <c r="F19" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F21" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G21" s="10" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
@@ -2064,17 +2225,11 @@
       <c r="E30" s="2"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="13"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A20:E20"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F1048576">

</xml_diff>

<commit_message>
Fundamentals Version 3 Commit. FINAL COMMIT FOR FUNDAMENTALS - add v3 code and comments - updated the spreadsheet with test cases - updated the output log with the test case output - added the v3 test case png screencap of console
</commit_message>
<xml_diff>
--- a/fundamentals-test-cases.xlsx
+++ b/fundamentals-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seneca\CPR101\CPR101-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315CD049-326E-4165-9D56-D1B9CA53EE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1F493B-2E8E-41D5-BA4F-BE497F9D2CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -789,7 +789,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
   <si>
     <t>Comments</t>
   </si>
@@ -1090,6 +1090,60 @@
   </si>
   <si>
     <t>The length of 'Q' is 1 characters</t>
+  </si>
+  <si>
+    <t>+Program handles expected input and runs as expected</t>
+  </si>
+  <si>
+    <t>+Program correctly handles a min length string</t>
+  </si>
+  <si>
+    <t>New destination string is 'Hello World'</t>
+  </si>
+  <si>
+    <t>New destination string is ''</t>
+  </si>
+  <si>
+    <t>New destination string is '1234567890123456789023456789012345678901234567890123456789012345678901234567890'</t>
+  </si>
+  <si>
+    <t>"12345678901234567890234567890123456789012345678901234567890123456789012345678901234567890"</t>
+  </si>
+  <si>
+    <t>Error: String length over buffer size</t>
+  </si>
+  <si>
+    <t>Program lost the last character and also overflowed. The reason is that the null terminator that is put in by fgets() overflowed the string. The final char '0' was overwritten by the manual null termination added and thus it interpreted the input as two strings, one being the original text missing the final char and an "empty" string with only the null terminator.
+Recommended Fix: Fixes for this issue are identical to ones mentioned in Version 1 and 2. Namely, start using safer input methods such as sscanf() and have the buffer be 1 larger than the max size. 
+It seems every version suffers from this same issue - they don't check for the size of the string before they parse it. This could easily be remedied but the code has not made an attempt unfortunately.</t>
+  </si>
+  <si>
+    <t>New destination string is '123456789012345678902345678901234567890123456789012345678901234567890123456789'
+Destination string is reset to empty
+Type the source string (q - to quit):
+New destination string is '1234567890'
+Destination string is reset to empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same issue as above unfortunately, but the cut off string was longer. This resulted in the overflow string containing the extra 10 chars that were added.
+Recommended Fix: Fixes for this issue are identical to above. Namely, start using safer input methods such as sscanf() and have the buffer be 1 larger than the max size. </t>
+  </si>
+  <si>
+    <t>+Program correctly handles a max length string</t>
+  </si>
+  <si>
+    <t>+Program correctly handles an overflowing string (too large)</t>
+  </si>
+  <si>
+    <t>New destination string is 'Q'
+Destination string is reset to empty</t>
+  </si>
+  <si>
+    <t>New destination string is '123456789012345678902345678901234567890123456789012345678901234567890123456789'
+Destination string is reset to empty
+Type the source string (q - to quit):
+New destination string is ''
+Destination string is reset to empty</t>
   </si>
 </sst>
 </file>
@@ -1401,21 +1455,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1428,7 +1479,10 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1736,8 +1790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1755,31 +1809,31 @@
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18" t="str" cm="1">
+      <c r="B1" s="17" t="str" cm="1">
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>Fundamentals</v>
       </c>
-      <c r="C1" s="24" t="str">
+      <c r="C1" s="23" t="str">
         <f ca="1">"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As Fundamentals_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1887,7 +1941,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1936,7 +1990,7 @@
       <c r="A10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1959,7 +2013,7 @@
       <c r="A11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="19" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1982,7 +2036,7 @@
       <c r="A12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="19" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1996,17 +2050,17 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2037,7 +2091,7 @@
       <c r="A15" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="20" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -2134,17 +2188,17 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2171,57 +2225,144 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
+    <row r="22" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
+      <c r="F22" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="E23" s="2"/>
-      <c r="F23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="13"/>
+      <c r="F23" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="357" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="191.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
-      <c r="B27" s="17"/>
+      <c r="A27" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="13"/>
+      <c r="F27" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="16"/>
-      <c r="B28" s="17"/>
+      <c r="B28" s="25"/>
       <c r="E28" s="2"/>
       <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="16"/>
-      <c r="B29" s="17"/>
+      <c r="B29" s="25"/>
       <c r="E29" s="2"/>
       <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
-      <c r="B30" s="17"/>
+      <c r="B30" s="25"/>
       <c r="E30" s="2"/>
       <c r="F30" s="13"/>
     </row>

</xml_diff>